<commit_message>
wait group for go routines
</commit_message>
<xml_diff>
--- a/p1_p2_p123_pnames2_goarchive.xlsx
+++ b/p1_p2_p123_pnames2_goarchive.xlsx
@@ -58,7 +58,7 @@
     <t>periode</t>
   </si>
   <si>
-    <t>name_1</t>
+    <t>name_3</t>
   </si>
   <si>
     <t>bonjour</t>
@@ -76,7 +76,7 @@
     <t>t3</t>
   </si>
   <si>
-    <t>name_4</t>
+    <t>name_5</t>
   </si>
   <si>
     <t>lll</t>

</xml_diff>